<commit_message>
Updated the same file
</commit_message>
<xml_diff>
--- a/lib/generators/spree_import_products/install/templates/sample.xlsx
+++ b/lib/generators/spree_import_products/install/templates/sample.xlsx
@@ -37,7 +37,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Autotelik:
+          <t xml:space="preserve">Spree_Edge:
 Required Field. 
 </t>
         </r>
@@ -65,7 +65,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Autotelik:
+          <t xml:space="preserve">Spree_Edge:
 Required Field. 
 </t>
         </r>
@@ -75,6 +75,16 @@
       <text>
         <r>
           <rPr>
+            <sz val="10"/>
+            <rFont val="Verdana"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Spree_Edge:
+</t>
+        </r>
+        <r>
+          <rPr>
             <sz val="8"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
@@ -97,7 +107,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Autotelik:
+          <t xml:space="preserve">Spree_Edge:
 </t>
         </r>
         <r>
@@ -134,14 +144,23 @@
       <text>
         <r>
           <rPr>
+            <sz val="10"/>
+            <rFont val="Verdana"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Spree_Edge:
+</t>
+        </r>
+        <r>
+          <rPr>
             <sz val="8"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Autotelik:
-The properties to associate with this product. 
+          <t xml:space="preserve">The properties to associate with this product. 
 Properties are for small snippets of text, shared across many products,
 and are for display purposes only. 
 An optional display value can be supplied to supplement the displayed text.
@@ -161,7 +180,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Autotelik:
+          <t xml:space="preserve">Spree_Edge:
 </t>
         </r>
         <r>
@@ -181,6 +200,16 @@
     </comment>
     <comment ref="K1" authorId="0">
       <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Verdana"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Spree_Edge:
+</t>
+        </r>
         <r>
           <rPr>
             <sz val="8"/>
@@ -208,7 +237,8 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Number of items in stock.
+          <t xml:space="preserve">Spree_Edge:
+Number of items in stock.
 When creating Variants, column can be used to set stock level for each option. In this situation make sure the count_on_hand column comes AFTER the Variants column, so that the variants have already been created. 
 Separate multiple values with </t>
         </r>
@@ -223,6 +253,20 @@
           </rPr>
           <t xml:space="preserve">|
 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Verdana"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Spree_Edge:
+Images will be seperated by pipe symbol, and the count of images will be same as the count of the images</t>
         </r>
       </text>
     </comment>
@@ -275,7 +319,7 @@
     <t xml:space="preserve">DEMO_001</t>
   </si>
   <si>
-    <t xml:space="preserve">Demo Product for AR Loader</t>
+    <t xml:space="preserve">Demo Product 1</t>
   </si>
   <si>
     <t xml:space="preserve">Chnaged description for updated testing</t>
@@ -327,6 +371,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">https://media.istockphoto.com/id/1340269597/photo/classic-vintage-muscle-car.webp?s=612x612&amp;w=is&amp;k=20&amp;c=KSm7mm02eA9w-Tea3lL1FVphub3FsYXz4fbhC5tOc8k</t>
     </r>
@@ -335,6 +380,7 @@
         <sz val="10"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">=|</t>
     </r>
@@ -344,6 +390,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">https://media.istockphoto.com/id/147461093/photo/sports-car-on-a-coastal-road.webp?s=612x612&amp;w=is&amp;k=20&amp;c=5bq0iSk4fctYKeOylCTRQV3LveT5OQZq-AlfBjg3J80</t>
     </r>
@@ -352,6 +399,7 @@
         <sz val="10"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">=|</t>
     </r>
@@ -361,6 +409,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">https://cdn.pixabay.com/photo/2016/11/22/23/44/porsche-1851246_960_720.jpg</t>
     </r>
@@ -369,7 +418,7 @@
     <t xml:space="preserve">DEMO_002</t>
   </si>
   <si>
-    <t xml:space="preserve">Demo Excel Load via Jruby</t>
+    <t xml:space="preserve">Demo Product 2</t>
   </si>
   <si>
     <t xml:space="preserve">less blah</t>
@@ -402,6 +451,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">https://cdn.pixabay.com/photo/2016/12/12/17/54/pontiac-trans-am-1970-1902256_960_720.jpg</t>
     </r>
@@ -410,6 +460,7 @@
         <sz val="10"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">|</t>
     </r>
@@ -419,6 +470,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">https://media.istockphoto.com/id/1340269597/photo/classic-vintage-muscle-car.webp?s=612x612&amp;w=is&amp;k=20&amp;c=KSm7mm02eA9w-Tea3lL1FVphub3FsYXz4fbhC5tOc8k</t>
     </r>
@@ -427,6 +479,7 @@
         <sz val="10"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">=|</t>
     </r>
@@ -436,6 +489,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">https://media.istockphoto.com/id/147461093/photo/sports-car-on-a-coastal-road.webp?s=612x612&amp;w=is&amp;k=20&amp;c=5bq0iSk4fctYKeOylCTRQV3LveT5OQZq-AlfBjg3J80</t>
     </r>
@@ -444,6 +498,7 @@
         <sz val="10"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">=</t>
     </r>
@@ -452,7 +507,7 @@
     <t xml:space="preserve">DEMO_003</t>
   </si>
   <si>
-    <t xml:space="preserve">Demo third row in future</t>
+    <t xml:space="preserve">Demo Product 3</t>
   </si>
   <si>
     <t xml:space="preserve">more blah blah</t>
@@ -483,7 +538,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.00"/>
     <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -526,12 +581,6 @@
       <name val="Verdana"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Verdana"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -668,12 +717,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -695,8 +744,8 @@
   </sheetPr>
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O4" activeCellId="0" sqref="O4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.05078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -798,11 +847,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="72.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="108.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="16" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="11" t="s">
@@ -826,7 +875,7 @@
       <c r="I3" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="J3" s="17" t="s">
         <v>31</v>
       </c>
       <c r="K3" s="14" t="s">
@@ -835,15 +884,15 @@
       <c r="L3" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="M3" s="17" t="s">
+      <c r="M3" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="72.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="108.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="16" t="s">
         <v>36</v>
       </c>
       <c r="C4" s="10" t="s">
@@ -867,7 +916,7 @@
       <c r="I4" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="J4" s="16" t="s">
+      <c r="J4" s="17" t="s">
         <v>41</v>
       </c>
       <c r="K4" s="10" t="s">
@@ -876,7 +925,7 @@
       <c r="L4" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="M4" s="17" t="s">
+      <c r="M4" s="15" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Variants with multiple images
</commit_message>
<xml_diff>
--- a/lib/generators/spree_import_products/install/templates/sample.xlsx
+++ b/lib/generators/spree_import_products/install/templates/sample.xlsx
@@ -37,7 +37,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Spree_Edge:
+          <t xml:space="preserve">Autotelik:
 Required Field. 
 </t>
         </r>
@@ -65,7 +65,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Spree_Edge:
+          <t xml:space="preserve">Autotelik:
 Required Field. 
 </t>
         </r>
@@ -75,16 +75,6 @@
       <text>
         <r>
           <rPr>
-            <sz val="10"/>
-            <rFont val="Verdana"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Spree_Edge:
-</t>
-        </r>
-        <r>
-          <rPr>
             <sz val="8"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
@@ -107,7 +97,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Spree_Edge:
+          <t xml:space="preserve">Autotelik:
 </t>
         </r>
         <r>
@@ -144,23 +134,14 @@
       <text>
         <r>
           <rPr>
-            <sz val="10"/>
-            <rFont val="Verdana"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Spree_Edge:
-</t>
-        </r>
-        <r>
-          <rPr>
             <sz val="8"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">The properties to associate with this product. 
+          <t xml:space="preserve">Autotelik:
+The properties to associate with this product. 
 Properties are for small snippets of text, shared across many products,
 and are for display purposes only. 
 An optional display value can be supplied to supplement the displayed text.
@@ -180,7 +161,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Spree_Edge:
+          <t xml:space="preserve">Autotelik:
 </t>
         </r>
         <r>
@@ -200,16 +181,6 @@
     </comment>
     <comment ref="K1" authorId="0">
       <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Verdana"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Spree_Edge:
-</t>
-        </r>
         <r>
           <rPr>
             <sz val="8"/>
@@ -237,8 +208,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Spree_Edge:
-Number of items in stock.
+          <t xml:space="preserve">Number of items in stock.
 When creating Variants, column can be used to set stock level for each option. In this situation make sure the count_on_hand column comes AFTER the Variants column, so that the variants have already been created. 
 Separate multiple values with </t>
         </r>
@@ -265,8 +235,29 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Spree_Edge:
-Images will be seperated by pipe symbol, and the count of images will be same as the count of the images</t>
+          <t xml:space="preserve">One can add multiple images to the variant.
+For ex:- 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="10"/>
+            <rFont val="Verdana"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">a,b,c| d,e,f
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Verdana"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Above line will produce 2 variants having 3 images each.</t>
         </r>
       </text>
     </comment>
@@ -319,7 +310,7 @@
     <t xml:space="preserve">DEMO_001</t>
   </si>
   <si>
-    <t xml:space="preserve">Demo Product 1</t>
+    <t xml:space="preserve">Demo Product for AR Loader</t>
   </si>
   <si>
     <t xml:space="preserve">Chnaged description for updated testing</t>
@@ -418,7 +409,7 @@
     <t xml:space="preserve">DEMO_002</t>
   </si>
   <si>
-    <t xml:space="preserve">Demo Product 2</t>
+    <t xml:space="preserve">Demo Excel Load via Jruby</t>
   </si>
   <si>
     <t xml:space="preserve">less blah</t>
@@ -507,7 +498,7 @@
     <t xml:space="preserve">DEMO_003</t>
   </si>
   <si>
-    <t xml:space="preserve">Demo Product 3</t>
+    <t xml:space="preserve">Demo third row in future</t>
   </si>
   <si>
     <t xml:space="preserve">more blah blah</t>
@@ -538,7 +529,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.00"/>
     <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -583,11 +574,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
@@ -652,7 +638,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -715,10 +701,6 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -744,8 +726,8 @@
   </sheetPr>
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.05078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -847,11 +829,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="108.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="72.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="10" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="11" t="s">
@@ -875,7 +857,7 @@
       <c r="I3" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="J3" s="16" t="s">
         <v>31</v>
       </c>
       <c r="K3" s="14" t="s">
@@ -888,11 +870,11 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="108.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="72.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="10" t="s">
         <v>36</v>
       </c>
       <c r="C4" s="10" t="s">
@@ -916,7 +898,7 @@
       <c r="I4" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="J4" s="17" t="s">
+      <c r="J4" s="16" t="s">
         <v>41</v>
       </c>
       <c r="K4" s="10" t="s">

</xml_diff>